<commit_message>
Mise à jour des fichers des recettes
</commit_message>
<xml_diff>
--- a/team/recettes/boeuf bourguignon.xlsx
+++ b/team/recettes/boeuf bourguignon.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salma\IdeaProjects\2022-groupe01\team\recettes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077F0A2F-AE4E-4930-AF2B-0DD3E2991C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9C064E-53CE-49A2-A2F9-4615BD1CA4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9492" yWindow="2616" windowWidth="13548" windowHeight="8880" xr2:uid="{30F09B77-A13F-44A4-B6ED-EEC177E0F21B}"/>
+    <workbookView xWindow="1776" yWindow="1776" windowWidth="13548" windowHeight="8880" xr2:uid="{30F09B77-A13F-44A4-B6ED-EEC177E0F21B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Nom</t>
   </si>
@@ -119,6 +120,9 @@
   </si>
   <si>
     <t>Boeuf bourguignon</t>
+  </si>
+  <si>
+    <t>Quantite</t>
   </si>
 </sst>
 </file>
@@ -470,18 +474,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{671BB7CB-0750-458C-BC69-662D0C43F787}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
+    <col min="2" max="3" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,104 +493,128 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8">
+        <v>600</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -742,18 +770,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -775,14 +803,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8935650D-14DC-4D11-809C-B7A3E6972D08}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33B7EB88-B318-485B-B95A-B7C859D51395}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -796,4 +816,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8935650D-14DC-4D11-809C-B7A3E6972D08}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>